<commit_message>
modification des reqêtes sqlite pour tenir compte nouvelle version de l'IG publisher (#255)
* Update ressource_fhir.md

* Update ressource_fhir.md

* Update ressource_fhir.md

* Update ressource_fhir.md

* Update ressource_fhir.md

* Update ressource_fhir.md

* Update ressource_fhir.md

* Update ressource_fhir.md

* Update ressource_fhir.md

* Update ressource_fhir.md

* Update ressource_fhir.md

* Update ressource_fhir.md

* Update ressource_fhir.md

* Update ressource_fhir.md

* Update ressource_fhir.md

* Update ressource_fhir.md

* Update ressource_fhir.md

* Update ressource_fhir.md

* Update index.md

* enlever les commentaires 5ef17d9e072cfc92e74a1876d94ecffe9b027055
</commit_message>
<xml_diff>
--- a/ig/CodeSystem-input-task-sdo-codesystem.xlsx
+++ b/ig/CodeSystem-input-task-sdo-codesystem.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>4.0.2-ballot-3</t>
+    <t>4.0.2</t>
   </si>
   <si>
     <t>Name</t>
@@ -45,7 +45,7 @@
     <t>Status</t>
   </si>
   <si>
-    <t>draft</t>
+    <t>active</t>
   </si>
   <si>
     <t>Experimental</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-04-30T08:40:24+00:00</t>
+    <t>2024-11-22T13:34:24+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
Préparation release 403 (#319)
* Prepa release 4.0.3

* Update release-notes.md

* Update release-notes.md 1bcfd3b28d32f78a2787b077edb810f626367761
</commit_message>
<xml_diff>
--- a/ig/CodeSystem-input-task-sdo-codesystem.xlsx
+++ b/ig/CodeSystem-input-task-sdo-codesystem.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>4.0.2</t>
+    <t>4.0.3</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-11-22T13:34:24+00:00</t>
+    <t>2025-01-30T16:13:12+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
release 406 (#348) 9e8d4ae9520bb956720be1577f4edf9299d0c4ff
</commit_message>
<xml_diff>
--- a/ig/CodeSystem-input-task-sdo-codesystem.xlsx
+++ b/ig/CodeSystem-input-task-sdo-codesystem.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>4.0.5</t>
+    <t>4.0.6</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-14T08:50:08+00:00</t>
+    <t>2025-12-15T14:49:50+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -81,7 +81,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Code System pour la définition des éléments spécifiques de input dans ressource SDOTask</t>
+    <t>Code System pour la définition des éléments spécifiques de input dans ressource ESMSTask</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>